<commit_message>
member payment testcase added
</commit_message>
<xml_diff>
--- a/Resources/AMap.xlsx
+++ b/Resources/AMap.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakshmi.saravanan\Desktop\selenium-adv1\Framework\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="5865" tabRatio="782" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="3495" tabRatio="782" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -20,6 +15,7 @@
     <sheet name="MemberPayment" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="176">
   <si>
     <t>Element_Name</t>
   </si>
@@ -551,6 +547,12 @@
   </si>
   <si>
     <t>#backToMemberProfileButton</t>
+  </si>
+  <si>
+    <t>BTN_Success_Submit</t>
+  </si>
+  <si>
+    <t>.//*[@id='tdContents']/form/table[1]/tbody/tr[2]/td/table/tbody/tr[7]/td/input</t>
   </si>
 </sst>
 </file>
@@ -1870,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" activeCellId="1" sqref="C15 C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,6 +2108,17 @@
         <v>173</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
member payment verification page object class
</commit_message>
<xml_diff>
--- a/Resources/AMap.xlsx
+++ b/Resources/AMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14565" windowHeight="5865" tabRatio="782" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="3255" tabRatio="782" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="182">
   <si>
     <t>Element_Name</t>
   </si>
@@ -544,6 +544,33 @@
   </si>
   <si>
     <t>html/body/div[2]/div/div/div/div[3]/table/tbody/tr[1]/td[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="tdContents"]/form/table[1]/tbody/tr[2]/td/table/tbody/tr[2]/td[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="tdContents"]/form/table[1]/tbody/tr[2]/td/table/tbody/tr[3]/td[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="tdContents"]/form/table[1]/tbody/tr[2]/td/table/tbody/tr[4]/td[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="tdContents"]/form/table[1]/tbody/tr[2]/td/table/tbody/tr[5]/td[2]</t>
+  </si>
+  <si>
+    <t>ELM_TransactionType</t>
+  </si>
+  <si>
+    <t>ELM_To</t>
+  </si>
+  <si>
+    <t>ELM_TransactionAmount</t>
+  </si>
+  <si>
+    <t>ELM_TransactionDescription</t>
+  </si>
+  <si>
+    <t>//*[@id="backButton"]</t>
   </si>
 </sst>
 </file>
@@ -1874,10 +1901,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,6 +2119,61 @@
         <v>170</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Account Balance Extract for single Account with verify account balance
</commit_message>
<xml_diff>
--- a/Resources/AMap.xlsx
+++ b/Resources/AMap.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohit_vora\Desktop\Selenium\Workspace\Framework\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumTestNg\Framework\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="3255" tabRatio="782" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="3255" tabRatio="782" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="189">
   <si>
     <t>Element_Name</t>
   </si>
@@ -578,12 +578,30 @@
   </si>
   <si>
     <t>input.button</t>
+  </si>
+  <si>
+    <t>ELM_SingleAccountPane</t>
+  </si>
+  <si>
+    <t>html/body/div[2]/div/div/div/div[3]/form/table/tbody/tr[1]/td[1]</t>
+  </si>
+  <si>
+    <t>html/body/div[2]/div/div/div/div[3]/table[1]/tbody/tr[2]/td/table/tbody/tr/td[1]</t>
+  </si>
+  <si>
+    <t>ELM_SingleAccountType</t>
+  </si>
+  <si>
+    <t>ELM_SingleAccountBalance</t>
+  </si>
+  <si>
+    <t>html/body/div[2]/div/div/div/div[3]/table[1]/tbody/tr[2]/td/table/tbody/tr/td[2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1047,17 +1065,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1139,6 +1157,39 @@
       </c>
       <c r="C5" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1904,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>